<commit_message>
Juhendtekstid ja mõned kosmeetilised parandused
</commit_message>
<xml_diff>
--- a/blocks1.xlsx
+++ b/blocks1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D781E35A-7AB5-41A9-970D-B9E0277F6FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{D781E35A-7AB5-41A9-970D-B9E0277F6FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55A46ED4-637D-48B7-9E36-C4BF389A4A46}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>intro_text_content</t>
   </si>
@@ -48,57 +48,50 @@
     <t>0:1</t>
   </si>
   <si>
-    <t>1:5</t>
-  </si>
-  <si>
-    <t>Enne katse lõpetamist küsime sinult veel mõned küsimused.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Punktide kogumine on lõppenud! </t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
-    <t>Sellega on katse lõppenud. 
-Vajuta noolele, et alustada andmete laadimist serverisse. 
-Kui see on lõppenud, avaneb uuringu küsimustiku osa.</t>
-  </si>
-  <si>
-    <t>Tere tulemast katsesse! 
+    <t>dif</t>
+  </si>
+  <si>
+    <t>outlier</t>
+  </si>
+  <si>
+    <t>0:0</t>
+  </si>
+  <si>
+    <t>Algamas on kognitiivse efektiivsuse katse. 
 Esmalt tutvustame sulle samm-sammult katse loogikat. 
-Jätkamiseks vajuta noolt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Katses ootavad loomist erineva raskusastmega kujundid. 
-Esmalt näed kujundit ekraanil, seejärel proovi see võimalikult täpselt järele joonistada. 
-Proovi esmalt kergema kujundi loomist. </t>
-  </si>
-  <si>
-    <t>Algab uus punktide kogumise seeria</t>
-  </si>
-  <si>
-    <t>dif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enne punktide kogumist saad katset veelkord harjutada. 
-Harjutusseeria lõpus näed ka tagasisidet oma soorituse kohta ja küsimusi, mida sinult katse jooksul küsitakse. </t>
-  </si>
-  <si>
-    <t>outlier</t>
-  </si>
-  <si>
-    <t>Nüüd näed ka tagasisidet enda soorituse kohta</t>
-  </si>
-  <si>
-    <t>0:0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selle katse eesmärk oli uurida võidust ja kaotusest tingitud emotsionaalsete seisundite mõju mälule. 
-Et võite ja kaotusi süstemaatiliselt manipuleerida, nägid sa tagasisidet oma soorituse kohta, mis ei vastanud tegelikkusele. </t>
-  </si>
-  <si>
-    <t>Nüüd saad proovida raskemate kujundite loomist</t>
+Sinu ülesandeks siin katses on arvutihiirega järele joonistada erinevaid kujundeid, mida sa mõneks sekundiks ekraanil näed. Püüa seda teha võimalikult täpselt aga samas ka võimalikult kiiresti. 
+Vajuta noolt, et seda ülesannet proovida.</t>
+  </si>
+  <si>
+    <t>Ilmselt märkasid ekraanil täpsuse ja kiiruse näidikuid. Täpsuse näidik annab teada, kui kaugel sa parasjagu kujundist oled. Kiiruse näidik loeb aega joonistamise algusest. 
+Sinu eesmärk on joonistada kujundeid võimalikult kiiresti ilma täpsuse näidikul suuri arve nägemata.
+Vajuta noolt, et ülesannet veelkord proovida.</t>
+  </si>
+  <si>
+    <t>Katses ootavad sind kahe erineva raskusastmega kujundid. Seni proovitud kujundid oli kergemad, nüüd saad proovida ka kahe raskema kujundi loomist.</t>
+  </si>
+  <si>
+    <t>Katse annab sulle aeg-ajalt ka tagasisidet sinu soorituse kohta.
+Täpsemalt näed, kuhu paigutuvad sinu sooritused selle katse soorituste normaaljaotuse suhtes.  Võrdlusandmed pärinevad sama katseparadigma kasutanud uuringutest USA-s.  
+Järgmise ülesande lõpus näed ka tagasisidet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katse jaguneb plokkideks, millest igaühes on 4 sama raskusastmega kujundit. Ploki lõpus näed tagasisidet kõigi nelja kujundi kohta.
+Pärast tagasiside nägemist esitatakse sulle ka mõned küsimused.
+Enne kognitiivse efektiivsuse mõõtmisega alustamist saad läbi teha ühe harjusploki. </t>
+  </si>
+  <si>
+    <t>Algab uus kognitiivse efektiivsuse mõõtmise plokk</t>
+  </si>
+  <si>
+    <t>Aitäh! Kognitiivse efektiivsuse mõõtmised on lõppenud. 
+Lõpetuseks küsime sinult veel mõned küsimused.</t>
+  </si>
+  <si>
+    <t>1:4</t>
   </si>
 </sst>
 </file>
@@ -434,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,10 +450,10 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -469,7 +462,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -478,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -489,36 +482,36 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -541,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -556,7 +549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -566,8 +559,8 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -579,10 +572,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -593,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -619,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -645,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -671,7 +664,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -697,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -712,9 +705,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -723,7 +716,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -732,88 +725,10 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uued tekstid koosolekult; VAS näidik halliks
</commit_message>
<xml_diff>
--- a/blocks1.xlsx
+++ b/blocks1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{D781E35A-7AB5-41A9-970D-B9E0277F6FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D55E173E-1CCF-4B99-B5BF-F7EC83D88F5D}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{D781E35A-7AB5-41A9-970D-B9E0277F6FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61D423F7-FCB2-46F2-9B88-AB316BC33297}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>intro_text_content</t>
   </si>
@@ -58,27 +58,6 @@
   </si>
   <si>
     <t>0:0</t>
-  </si>
-  <si>
-    <t>Ilmselt märkasid ekraanil täpsuse ja kiiruse näidikuid. Täpsuse näidik annab teada, kui kaugel sa parasjagu kujundist oled. Kiiruse näidik loeb aega joonistamise algusest. 
-Sinu eesmärk on joonistada kujundeid võimalikult kiiresti ilma täpsuse näidikul suuri arve nägemata.
-Vajuta noolt, et ülesannet veelkord proovida.</t>
-  </si>
-  <si>
-    <t>Katses ootavad sind kahe erineva raskusastmega kujundid. Seni proovitud kujundid oli kergemad, nüüd saad proovida ka kahe raskema kujundi loomist.</t>
-  </si>
-  <si>
-    <t>Katse annab sulle aeg-ajalt ka tagasisidet sinu soorituse kohta.
-Täpsemalt näed, kuhu paigutuvad sinu sooritused selle katse soorituste normaaljaotuse suhtes.  Võrdlusandmed pärinevad sama katseparadigma kasutanud uuringutest USA-s.  
-Järgmise ülesande lõpus näed ka tagasisidet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Katse jaguneb plokkideks, millest igaühes on 4 sama raskusastmega kujundit. Ploki lõpus näed tagasisidet kõigi nelja kujundi kohta.
-Pärast tagasiside nägemist esitatakse sulle ka mõned küsimused.
-Enne kognitiivse efektiivsuse mõõtmisega alustamist saad läbi teha ühe harjusploki. </t>
-  </si>
-  <si>
-    <t>Algab uus kognitiivse efektiivsuse mõõtmise plokk</t>
   </si>
   <si>
     <t>Aitäh! Kognitiivse efektiivsuse mõõtmised on lõppenud. 
@@ -88,10 +67,46 @@
     <t>1:4</t>
   </si>
   <si>
-    <t>Algamas on kognitiivse efektiivsuse katse. Esmalt tutvustame sulle samm-sammult katse loogikat. 
-Sinu ülesandeks siin katses on arvutihiirega järele joonistada erinevaid kujundeid, mida sa mõneks sekundiks ekraanil näed. Püüa seda teha võimalikult täpselt ja ka võimalikult kiiresti. 
-Et juhuslikud vead su tulemust ei mõjutaks, saad sa alati uue katse kui käimasolev ilmselgelt ebaõnnestub.
+    <t>Katses ootavad sind kahe erineva raskusastmega kujundid. Seni proovitud kujundid oli kergemad, nüüd saad proovida ka kahe raskema kujundi loomist. Kujundi rasksuastmest annab märku kujundi värv.</t>
+  </si>
+  <si>
+    <t>Kognitiivse efektiivsuse mõõtmise plokk: 1
+Pea meeles, et oluline on nii täpsus kui kiirus.</t>
+  </si>
+  <si>
+    <t>Kognitiivse efektiivsuse mõõtmise plokk: 2
+Pea meeles, et oluline on nii täpsus kui kiirus.</t>
+  </si>
+  <si>
+    <t>Kognitiivse efektiivsuse mõõtmise plokk: 3
+Pea meeles, et oluline on nii täpsus kui kiirus.</t>
+  </si>
+  <si>
+    <t>Kognitiivse efektiivsuse mõõtmise plokk: 4
+Pea meeles, et oluline on nii täpsus kui kiirus.</t>
+  </si>
+  <si>
+    <t>Algav katse mõõdab sinu kognitiivset efektiivsust. Kognitiivne efektiivsus on uudne suund vaimse võimekuse määratlemisel, mis lähtub eeldusest, et psüühika evolutsiooniline ülesanne on töödelda infot käitumise juhtimiseks. Kognitiivne efektiivsus viitab selle protsess kui terviku tõhususele, eristudes nii alternatiivsetest vaimse võimekuse käsitlustest, mis keskenduvad kitsamalt info töötlemisele. Algav katse on üks paljudest vahenditest, mida uurijad kognitiivse efektiivsuse mõõtmiseks on välja arendamas. 
+Esmalt tutvustame sulle samm-sammult katse loogikat. 
+Sinu ülesandeks siin katses on arvutihiirega järele joonistada erinevaid kujundeid. Püüa seda teha võimalikult täpselt ja ka võimalikult kiiresti. 
+Et kui mõni katse ilmselgelt ebaõnnestub, saad uue võimaluse.
 Vajuta noolt, et ülesannet proovida.</t>
+  </si>
+  <si>
+    <t>Võib-olla märkasid ekraanil täpsuse ja kestuse näidikuid. Täpsuse näidik annab teada, kui kaugel su hiir kujundist parasjagu on. Kestuse näidik loeb aega joonistamise algusest. 
+Sinu eesmärk on joonistada kujundeid võimalikult täpselt ja ka võimalikult kiiresti.
+Vajuta noolt, et ülesannet veelkord proovida.</t>
+  </si>
+  <si>
+    <t>Katses kuvatakse aeg-ajalt tagasisidet sinu soorituse kohta.
+Täpsemalt näed, mitmest protsentist inimestest sinu sooritus tõenäoliselt parem oli. Võrdlusandmed pärinevad sama katseparadigma kasutanud uuringutest USA-s.
+Järgmise ülesande lõpus näed ka tagasisidet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katse jaguneb plokkideks. Igas plokis on 4 sama raskusastmega kujundit. 
+Iga ploki lõpus näed tagasisidet kõigi nelja soorituse kohta. Pane tähele, et tagasiside on järjestatud mitte kujundite esitamise vaid soorituse kvaliteedi alusel.
+Pärast tagasisidet palutakse sul hinnata, millise tunde plokis saadud tulemus tekitas. 
+Enne mõõtmisega alustamist saad läbi teha ühe harjutusploki. </t>
   </si>
 </sst>
 </file>
@@ -429,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -508,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -523,7 +538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -533,8 +548,8 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -560,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -575,7 +590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -586,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -601,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -612,7 +627,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -627,7 +642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -653,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -664,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -679,7 +694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -690,7 +705,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -707,17 +722,17 @@
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E11">
         <v>0</v>
       </c>
@@ -728,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rec cols in conditions and video size
</commit_message>
<xml_diff>
--- a/blocks1.xlsx
+++ b/blocks1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56DBE82-D9B0-430A-AB8C-EFAFD6573531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509F121B-149A-4671-9F48-AE96E7BDA290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>intro_text_content</t>
   </si>
@@ -107,6 +107,9 @@
 Sinu ülesandeks siin katses on arvutihiirega järele joonistada erinevaid kujundeid. Püüa seda teha võimalikult täpselt ja ka võimalikult kiiresti. 
 Et kui mõni katse ilmselgelt ebaõnnestub, saad uue võimaluse.
 Vajuta noolt, et ülesannet proovida.</t>
+  </si>
+  <si>
+    <t>videoRec</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +463,7 @@
     <col min="8" max="8" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -485,8 +488,11 @@
       <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -511,8 +517,11 @@
       <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -537,8 +546,11 @@
       <c r="H3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -563,8 +575,11 @@
       <c r="H4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -589,8 +604,11 @@
       <c r="H5" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -615,8 +633,11 @@
       <c r="H6" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -641,8 +662,11 @@
       <c r="H7" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -667,8 +691,11 @@
       <c r="H8" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -693,8 +720,11 @@
       <c r="H9" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -719,8 +749,11 @@
       <c r="H10" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -744,6 +777,9 @@
       </c>
       <c r="H11" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>